<commit_message>
Updated report generation functionality
</commit_message>
<xml_diff>
--- a/src/test/resource/resources/TestData.xlsx
+++ b/src/test/resource/resources/TestData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Software\SeleniumWorkspace\Ecommerce_App_automation\src\test\resource\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Software\SeleniumProjectWorkspace\TestNGWorkspace\Ecommerce_App_TestNG_Automation\src\test\resource\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BA60C18-8377-4E5E-865C-EBEF6EB22B55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E123631-A2AE-492E-931D-75A0E1D550A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,12 +25,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="2">
   <si>
     <t>ExpectedItemsList</t>
-  </si>
-  <si>
-    <t>ADIDAS ORIGINAL,ZARA COAT 3,IPHONE 13 PRO</t>
   </si>
   <si>
     <t>ADIDAS ORIGINAL,IPHONE 13 PRO</t>
@@ -363,7 +360,7 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -385,7 +382,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>